<commit_message>
Updated Project frontend and backend
</commit_message>
<xml_diff>
--- a/Project/Bug-Tracking-System/API-Docs.xlsx
+++ b/Project/Bug-Tracking-System/API-Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/presidio/Documents/Repo/june6-project/Bug-Tracking-System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C22EEB-EA42-C141-9282-EB243790E474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4408FA-B4A1-FA49-9518-0162DF47BBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{5F4BF89F-5E06-E74D-B5C7-1FAAEA842B43}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="21320" windowHeight="22400" xr2:uid="{5F4BF89F-5E06-E74D-B5C7-1FAAEA842B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Query (3)" sheetId="4" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Anyone</t>
   </si>
   <si>
-    <t>Tester</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>/api/v1/Bugs/status?BugId=3</t>
+  </si>
+  <si>
+    <t>Tester,Admin</t>
   </si>
 </sst>
 </file>
@@ -511,21 +511,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -594,6 +579,21 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="22"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
@@ -615,14 +615,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D66F7FD0-13A0-2444-8DEA-2C527357F1F8}" name="Query__3" displayName="Query__3" ref="C1:G1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D66F7FD0-13A0-2444-8DEA-2C527357F1F8}" name="Query__3" displayName="Query__3" ref="C1:G1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="C1:G1048576" xr:uid="{D66F7FD0-13A0-2444-8DEA-2C527357F1F8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{81AFD494-74D8-4240-B347-3F707005F21F}" name="Method" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{33138300-3553-5A46-8EE0-B0A8931B6E46}" name="Endpoints" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{E463F368-007F-F14B-861B-2534BF7EB168}" name="Access" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{40F03577-BB1A-6449-B9DE-7F54273C5092}" name="Example Request" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{BADD02CD-59DF-EC41-AE5B-5E1C47D9FDB6}" name=" Example Response" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{81AFD494-74D8-4240-B347-3F707005F21F}" name="Method" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{33138300-3553-5A46-8EE0-B0A8931B6E46}" name="Endpoints" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E463F368-007F-F14B-861B-2534BF7EB168}" name="Access" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{40F03577-BB1A-6449-B9DE-7F54273C5092}" name="Example Request" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{BADD02CD-59DF-EC41-AE5B-5E1C47D9FDB6}" name=" Example Response" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915E0EED-284D-8243-9E7D-5B661E9649CD}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -978,24 +978,24 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="175" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
@@ -1004,15 +1004,15 @@
         <v>17</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="175" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>1</v>
@@ -1021,15 +1021,15 @@
         <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="150" x14ac:dyDescent="0.35">
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>2</v>
@@ -1038,15 +1038,15 @@
         <v>18</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="75" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>3</v>
@@ -1055,15 +1055,15 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="100" x14ac:dyDescent="0.35">
       <c r="C6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
@@ -1072,12 +1072,12 @@
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="150" x14ac:dyDescent="0.35">
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>5</v>
@@ -1086,15 +1086,15 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="75" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>6</v>
@@ -1103,32 +1103,32 @@
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="325" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1137,30 +1137,30 @@
         <v>18</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="409.6" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>10</v>
@@ -1169,32 +1169,32 @@
         <v>17</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="409.6" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="150" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>12</v>
@@ -1203,12 +1203,12 @@
         <v>17</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="200" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>13</v>
@@ -1217,12 +1217,12 @@
         <v>18</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="200" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>14</v>
@@ -1231,12 +1231,12 @@
         <v>17</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>15</v>
@@ -1245,27 +1245,27 @@
         <v>17</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="275" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
@@ -1297,13 +1297,13 @@
   <sheetData>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>